<commit_message>
tarea 9 corrección solución  varianza suma
</commit_message>
<xml_diff>
--- a/Problemas/V.A. Discreta bidimensionales/problema_ACCIONES.xlsx
+++ b/Problemas/V.A. Discreta bidimensionales/problema_ACCIONES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t169\Documents\CURSOS\pe4b\pe4b\Problemas\V.A. Discreta bidimensionales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CC67D9-F024-4894-A82F-AFB97F6588E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2667A6A-CE6C-455D-A398-019DC28C8021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,7 +924,7 @@
   <dimension ref="A2:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>